<commit_message>
add my lab task
</commit_message>
<xml_diff>
--- a/Mooncity.xlsx
+++ b/Mooncity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\V530-Computing\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eunom\Desktop\cst导论\LAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6BCD52-2665-4F04-95B8-640B2684AECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400D1D94-7A95-4F34-A699-7AE256EC2498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{7DA16BB4-1FF7-4591-891F-93558EAF8FA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7DA16BB4-1FF7-4591-891F-93558EAF8FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,18 +137,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -185,7 +185,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,7 +203,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -274,7 +274,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -438,6 +438,31 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>DAY</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -463,7 +488,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -495,7 +520,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="689058864"/>
@@ -546,9 +571,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-MY"/>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
                   <a:t>RAINFALL(mm)</a:t>
                 </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -577,7 +603,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -609,7 +635,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="689061424"/>
@@ -624,37 +650,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -688,7 +683,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1275,7 +1270,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1573,21 +1568,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439BBF51-28F0-4038-B908-4589292EE581}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1622,7 +1617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1661,12 +1656,12 @@
         <v>18.571428571428573</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1">
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1716,7 +1711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>

</xml_diff>